<commit_message>
Updating so that only missing values can be recorded for the YES PHN subscales. This is being put in place until AIHW have reviewed the calculation of the subscales.
</commit_message>
<xml_diff>
--- a/doc/_static/example-files/PMHC-MDS-Survey-1-0-delete.xlsx
+++ b/doc/_static/example-files/PMHC-MDS-Survey-1-0-delete.xlsx
@@ -970,10 +970,10 @@
         <v>1</v>
       </c>
       <c r="AH2">
-        <v>36</v>
+        <v>99</v>
       </c>
       <c r="AI2">
-        <v>9</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:36">
@@ -1068,10 +1068,10 @@
         <v>2</v>
       </c>
       <c r="AH3">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="AI3">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="AJ3" t="s">
         <v>68</v>

</xml_diff>